<commit_message>
unified report and thesis documents
</commit_message>
<xml_diff>
--- a/results_crossentropy.xlsx
+++ b/results_crossentropy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001149822\personal\teseMECD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCB0791-CD85-498F-AD21-18F5C630D920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED9F735-A918-43E7-946C-E8203AF8E7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,11 +697,11 @@
       </c>
       <c r="E16">
         <f>MAX(B16:B20)</f>
-        <v>0.73501733531451197</v>
+        <v>0.76374442793462105</v>
       </c>
       <c r="F16">
         <f>AVERAGE(B16:B20)</f>
-        <v>0.73501733531451197</v>
+        <v>0.75443288756810267</v>
       </c>
       <c r="G16">
         <f>MIN(C16:C20)</f>
@@ -709,39 +709,63 @@
       </c>
       <c r="H16">
         <f>MAX(C16:C20)</f>
-        <v>0.72700296735905001</v>
+        <v>0.764589515331355</v>
       </c>
       <c r="I16">
         <f>AVERAGE(C16:C20)</f>
-        <v>0.72700296735905001</v>
+        <v>0.74540059347180965</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
+      <c r="B17">
+        <v>0.75482912332838004</v>
+      </c>
+      <c r="C17">
+        <v>0.764589515331355</v>
+      </c>
       <c r="F17">
         <f>MAX(F16-D16,E16-F16)</f>
-        <v>0</v>
+        <v>1.9415552253590707E-2</v>
       </c>
       <c r="I17">
         <f>MAX(H16-I16,I16-G16)</f>
-        <v>0</v>
+        <v>1.9188921859545349E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
+      <c r="B18">
+        <v>0.75928677563150004</v>
+      </c>
+      <c r="C18">
+        <v>0.74085064292779401</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
+      <c r="B19">
+        <v>0.75928677563150004</v>
+      </c>
+      <c r="C19">
+        <v>0.75865479723046403</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0.76374442793462105</v>
+      </c>
+      <c r="C20">
+        <v>0.73590504451038496</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
new results transfer learning
</commit_message>
<xml_diff>
--- a/results_crossentropy.xlsx
+++ b/results_crossentropy.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001149822\personal\teseMECD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED9F735-A918-43E7-946C-E8203AF8E7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175079AD-1583-48E7-B524-9EFFC95BA838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3 trials both models" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
   <si>
     <t>Run#1</t>
   </si>
@@ -87,6 +88,33 @@
   </si>
   <si>
     <t>Type - All samples Extension Positives Negatives (size 16640)</t>
+  </si>
+  <si>
+    <t>Type - Logical Augmentation LXMERT</t>
+  </si>
+  <si>
+    <t>Type - Logical Augmentation VILT</t>
+  </si>
+  <si>
+    <t>Type - Image Augmentation LXMERT</t>
+  </si>
+  <si>
+    <t>Type - Image Augmentation VILT</t>
+  </si>
+  <si>
+    <t>Type - Contrastive LXMERT</t>
+  </si>
+  <si>
+    <t>Type - Contrastive VILT</t>
+  </si>
+  <si>
+    <t>Type - Contrastive LXMERT Trial 2</t>
+  </si>
+  <si>
+    <t>Type - SNLI-VE Pretraining LXMERT</t>
+  </si>
+  <si>
+    <t>Type - SNLI-VE Finetuning LXMERT</t>
   </si>
 </sst>
 </file>
@@ -406,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -887,4 +915,825 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC7418E-5114-4E07-B454-35F017667A5A}">
+  <dimension ref="A1:S39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="53.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>77.31</v>
+      </c>
+      <c r="C2">
+        <v>75.77</v>
+      </c>
+      <c r="D2">
+        <f>MIN(B2:B6)</f>
+        <v>77.31</v>
+      </c>
+      <c r="E2">
+        <f>MAX(B2:B6)</f>
+        <v>78.31</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(B2:B6)</f>
+        <v>77.843333333333334</v>
+      </c>
+      <c r="G2">
+        <f>MIN(C2:C6)</f>
+        <v>75.77</v>
+      </c>
+      <c r="H2">
+        <f>MAX(C2:C6)</f>
+        <v>77.05</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(C2:C6)</f>
+        <v>76.623333333333335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>77.91</v>
+      </c>
+      <c r="C3">
+        <v>77.05</v>
+      </c>
+      <c r="F3">
+        <f>MAX(F2-D2,E2-F2)</f>
+        <v>0.53333333333333144</v>
+      </c>
+      <c r="I3">
+        <f>MAX(H2-I2,I2-G2)</f>
+        <v>0.85333333333333883</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>78.31</v>
+      </c>
+      <c r="C4">
+        <v>77.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>74.84</v>
+      </c>
+      <c r="C7">
+        <v>73.290000000000006</v>
+      </c>
+      <c r="D7">
+        <f>MIN(B7:B11)</f>
+        <v>73.84</v>
+      </c>
+      <c r="E7">
+        <f>MAX(B7:B11)</f>
+        <v>74.84</v>
+      </c>
+      <c r="F7">
+        <f>AVERAGE(B7:B11)</f>
+        <v>74.260000000000005</v>
+      </c>
+      <c r="G7">
+        <f>MIN(C7:C11)</f>
+        <v>73.290000000000006</v>
+      </c>
+      <c r="H7">
+        <f>MAX(C7:C11)</f>
+        <v>73.39</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(C7:C11)</f>
+        <v>73.356666666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>73.84</v>
+      </c>
+      <c r="C8">
+        <v>73.39</v>
+      </c>
+      <c r="F8">
+        <f>MAX(F7-D7,E7-F7)</f>
+        <v>0.57999999999999829</v>
+      </c>
+      <c r="I8">
+        <f>MAX(H7-I7,I7-G7)</f>
+        <v>6.6666666666662877E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="C9">
+        <v>73.39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>75.28</v>
+      </c>
+      <c r="C12">
+        <v>71.81</v>
+      </c>
+      <c r="D12">
+        <f>MIN(B12:B16)</f>
+        <v>75.28</v>
+      </c>
+      <c r="E12">
+        <f>MAX(B12:B16)</f>
+        <v>76.569999999999993</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(B12:B16)</f>
+        <v>76.089999999999989</v>
+      </c>
+      <c r="G12">
+        <f>MIN(C12:C16)</f>
+        <v>71.81</v>
+      </c>
+      <c r="H12">
+        <f>MAX(C12:C16)</f>
+        <v>73.89</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(C12:C16)</f>
+        <v>72.866666666666674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>76.42</v>
+      </c>
+      <c r="C13">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F13">
+        <f>MAX(F12-D12,E12-F12)</f>
+        <v>0.80999999999998806</v>
+      </c>
+      <c r="I13">
+        <f>MAX(H12-I12,I12-G12)</f>
+        <v>1.056666666666672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>76.569999999999993</v>
+      </c>
+      <c r="C14">
+        <v>73.89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>MIN(B17:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>MAX(B17:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" t="e">
+        <f>AVERAGE(B17:B21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17">
+        <f>MIN(C17:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>MAX(C17:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" t="e">
+        <f>AVERAGE(C17:C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="e">
+        <f>MAX(F17-D17,E17-F17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f>MAX(H17-I17,I17-G17)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="C22">
+        <v>75.67</v>
+      </c>
+      <c r="D22">
+        <f>MIN(B22:B26)</f>
+        <v>77.27</v>
+      </c>
+      <c r="E22">
+        <f>MAX(B22:B26)</f>
+        <v>79</v>
+      </c>
+      <c r="F22">
+        <f>AVERAGE(B22:B26)</f>
+        <v>77.909999999999982</v>
+      </c>
+      <c r="G22">
+        <f>MIN(C22:C26)</f>
+        <v>75.67</v>
+      </c>
+      <c r="H22">
+        <f>MAX(C22:C26)</f>
+        <v>76.849999999999994</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(C22:C26)</f>
+        <v>76.326666666666654</v>
+      </c>
+      <c r="K22" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0.78504210004952901</v>
+      </c>
+      <c r="M22">
+        <v>0.76755687438179998</v>
+      </c>
+      <c r="N22">
+        <f>MIN(L22:L26)</f>
+        <v>0.77513620604259503</v>
+      </c>
+      <c r="O22">
+        <f>MAX(L22:L26)</f>
+        <v>0.78504210004952901</v>
+      </c>
+      <c r="P22">
+        <f>AVERAGE(L22:L26)</f>
+        <v>0.77992405481261307</v>
+      </c>
+      <c r="Q22">
+        <f>MIN(M22:M26)</f>
+        <v>0.75173095944609303</v>
+      </c>
+      <c r="R22">
+        <f>MAX(M22:M26)</f>
+        <v>0.76755687438179998</v>
+      </c>
+      <c r="S22">
+        <f>AVERAGE(M22:M26)</f>
+        <v>0.76063303659742798</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="F23">
+        <f>MAX(F22-D22,E22-F22)</f>
+        <v>1.0900000000000176</v>
+      </c>
+      <c r="I23">
+        <f>MAX(H22-I22,I22-G22)</f>
+        <v>0.65666666666665208</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>0.77959385834571504</v>
+      </c>
+      <c r="M23">
+        <v>0.76261127596439104</v>
+      </c>
+      <c r="P23">
+        <f>MAX(P22-N22,O22-P22)</f>
+        <v>5.1180452369159468E-3</v>
+      </c>
+      <c r="S23">
+        <f>MAX(R22-S22,S22-Q22)</f>
+        <v>8.9020771513349528E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>77.27</v>
+      </c>
+      <c r="C24">
+        <v>76.459999999999994</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>0.77513620604259503</v>
+      </c>
+      <c r="M24">
+        <v>0.75173095944609303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>MIN(B27:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>MAX(B27:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" t="e">
+        <f>AVERAGE(B27:B31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27">
+        <f>MIN(C27:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>MAX(C27:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" t="e">
+        <f>AVERAGE(C27:C31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="e">
+        <f>MAX(F27-D27,E27-F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f>MAX(H27-I27,I27-G27)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>75.45</v>
+      </c>
+      <c r="C32">
+        <v>75.88</v>
+      </c>
+      <c r="D32">
+        <f>MIN(B32:B36)</f>
+        <v>75.290000000000006</v>
+      </c>
+      <c r="E32">
+        <f>MAX(B32:B36)</f>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="F32">
+        <f>AVERAGE(B32:B36)</f>
+        <v>75.446666666666673</v>
+      </c>
+      <c r="G32">
+        <f>MIN(C32:C36)</f>
+        <v>75.88</v>
+      </c>
+      <c r="H32">
+        <f>MAX(C32:C36)</f>
+        <v>76.12</v>
+      </c>
+      <c r="I32">
+        <f>AVERAGE(C32:C36)</f>
+        <v>75.993333333333339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="C33">
+        <v>75.98</v>
+      </c>
+      <c r="F33">
+        <f>MAX(F32-D32,E32-F32)</f>
+        <v>0.15666666666666629</v>
+      </c>
+      <c r="I33">
+        <f>MAX(H32-I32,I32-G32)</f>
+        <v>0.12666666666666515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>75.290000000000006</v>
+      </c>
+      <c r="C34">
+        <v>76.12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="C37">
+        <v>76.239999999999995</v>
+      </c>
+      <c r="D37">
+        <f>MIN(B37:B41)</f>
+        <v>74.84</v>
+      </c>
+      <c r="E37">
+        <f>MAX(B37:B41)</f>
+        <v>75.12</v>
+      </c>
+      <c r="F37">
+        <f>AVERAGE(B37:B41)</f>
+        <v>75</v>
+      </c>
+      <c r="G37">
+        <f>MIN(C37:C41)</f>
+        <v>75.900000000000006</v>
+      </c>
+      <c r="H37">
+        <f>MAX(C37:C41)</f>
+        <v>76.239999999999995</v>
+      </c>
+      <c r="I37">
+        <f>AVERAGE(C37:C41)</f>
+        <v>76.11333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>74.84</v>
+      </c>
+      <c r="C38">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="F38">
+        <f>MAX(F37-D37,E37-F37)</f>
+        <v>0.15999999999999659</v>
+      </c>
+      <c r="I38">
+        <f>MAX(H37-I37,I37-G37)</f>
+        <v>0.21333333333332405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>75.12</v>
+      </c>
+      <c r="C39">
+        <v>76.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
thesis new version and results new way
</commit_message>
<xml_diff>
--- a/results_crossentropy.xlsx
+++ b/results_crossentropy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001149822\personal\teseMECD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE750DA9-7D78-432C-B3A1-F56FFD41EB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E3805-FFA7-409D-8626-9111FE6B9CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="30">
   <si>
     <t>Run#1</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Type - SNLI-VE Finetuning LXMERT</t>
+  </si>
+  <si>
+    <t>Type - Logical Augmentation LXMERT new way</t>
+  </si>
+  <si>
+    <t>Type - Contrastive LXMERT new way 0.01</t>
+  </si>
+  <si>
+    <t>Type - Contrastive LXMERT new way 0.05</t>
+  </si>
+  <si>
+    <t>Type - Contrastive LXMERT new way 0.1</t>
   </si>
 </sst>
 </file>
@@ -919,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC7418E-5114-4E07-B454-35F017667A5A}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1645,7 +1657,7 @@
         <v>75.993333333333339</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>0.12666666666666515</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1675,7 +1687,7 @@
         <v>76.12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1704,7 +1716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1751,7 @@
         <v>76.11333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1758,7 +1770,7 @@
         <v>0.21333333333332405</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1767,6 +1779,366 @@
       </c>
       <c r="C39">
         <v>76.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>77.37</v>
+      </c>
+      <c r="C42">
+        <v>74.48</v>
+      </c>
+      <c r="D42">
+        <f>MIN(B42:B46)</f>
+        <v>77.37</v>
+      </c>
+      <c r="E42">
+        <f>MAX(B42:B46)</f>
+        <v>78.45</v>
+      </c>
+      <c r="F42">
+        <f>AVERAGE(B42:B46)</f>
+        <v>78.06</v>
+      </c>
+      <c r="G42">
+        <f>MIN(C42:C46)</f>
+        <v>74.48</v>
+      </c>
+      <c r="H42">
+        <f>MAX(C42:C46)</f>
+        <v>77.25</v>
+      </c>
+      <c r="I42">
+        <f>AVERAGE(C42:C46)</f>
+        <v>76.096666666666678</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>78.36</v>
+      </c>
+      <c r="C43">
+        <v>76.56</v>
+      </c>
+      <c r="F43">
+        <f>MAX(F42-D42,E42-F42)</f>
+        <v>0.68999999999999773</v>
+      </c>
+      <c r="I43">
+        <f>MAX(H42-I42,I42-G42)</f>
+        <v>1.6166666666666742</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>78.45</v>
+      </c>
+      <c r="C44">
+        <v>77.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" t="s">
+        <v>6</v>
+      </c>
+      <c r="N46" t="s">
+        <v>9</v>
+      </c>
+      <c r="O46" t="s">
+        <v>8</v>
+      </c>
+      <c r="P46" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>7</v>
+      </c>
+      <c r="R46" t="s">
+        <v>11</v>
+      </c>
+      <c r="S46" t="s">
+        <v>12</v>
+      </c>
+      <c r="U46" t="s">
+        <v>29</v>
+      </c>
+      <c r="V46" t="s">
+        <v>3</v>
+      </c>
+      <c r="W46" t="s">
+        <v>6</v>
+      </c>
+      <c r="X46" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>78.11</v>
+      </c>
+      <c r="C47">
+        <v>76.760000000000005</v>
+      </c>
+      <c r="D47">
+        <f>MIN(B47:B51)</f>
+        <v>77.41</v>
+      </c>
+      <c r="E47">
+        <f>MAX(B47:B51)</f>
+        <v>78.11</v>
+      </c>
+      <c r="F47">
+        <f>AVERAGE(B47:B51)</f>
+        <v>77.659999999999982</v>
+      </c>
+      <c r="G47">
+        <f>MIN(C47:C51)</f>
+        <v>76.760000000000005</v>
+      </c>
+      <c r="H47">
+        <f>MAX(C47:C51)</f>
+        <v>77.94</v>
+      </c>
+      <c r="I47">
+        <f>AVERAGE(C47:C51)</f>
+        <v>77.38333333333334</v>
+      </c>
+      <c r="K47" t="s">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>77.56</v>
+      </c>
+      <c r="M47">
+        <v>77.650000000000006</v>
+      </c>
+      <c r="N47">
+        <f>MIN(L47:L51)</f>
+        <v>76.97</v>
+      </c>
+      <c r="O47">
+        <f>MAX(L47:L51)</f>
+        <v>77.66</v>
+      </c>
+      <c r="P47">
+        <f>AVERAGE(L47:L51)</f>
+        <v>77.396666666666661</v>
+      </c>
+      <c r="Q47">
+        <f>MIN(M47:M51)</f>
+        <v>76.06</v>
+      </c>
+      <c r="R47">
+        <f>MAX(M47:M51)</f>
+        <v>77.650000000000006</v>
+      </c>
+      <c r="S47">
+        <f>AVERAGE(M47:M51)</f>
+        <v>76.69</v>
+      </c>
+      <c r="U47" t="s">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="W47">
+        <v>76.66</v>
+      </c>
+      <c r="X47">
+        <f>MIN(V47:V51)</f>
+        <v>77.459999999999994</v>
+      </c>
+      <c r="Y47">
+        <f>MAX(V47:V51)</f>
+        <v>78.599999999999994</v>
+      </c>
+      <c r="Z47">
+        <f>AVERAGE(V47:V51)</f>
+        <v>78.040000000000006</v>
+      </c>
+      <c r="AA47">
+        <f>MIN(W47:W51)</f>
+        <v>74.88</v>
+      </c>
+      <c r="AB47">
+        <f>MAX(W47:W51)</f>
+        <v>77.25</v>
+      </c>
+      <c r="AC47">
+        <f>AVERAGE(W47:W51)</f>
+        <v>76.263333333333335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>77.41</v>
+      </c>
+      <c r="C48">
+        <v>77.45</v>
+      </c>
+      <c r="F48">
+        <f>MAX(F47-D47,E47-F47)</f>
+        <v>0.45000000000001705</v>
+      </c>
+      <c r="I48">
+        <f>MAX(H47-I47,I47-G47)</f>
+        <v>0.62333333333333485</v>
+      </c>
+      <c r="K48" t="s">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>77.66</v>
+      </c>
+      <c r="M48">
+        <v>76.36</v>
+      </c>
+      <c r="P48">
+        <f>MAX(P47-N47,O47-P47)</f>
+        <v>0.42666666666666231</v>
+      </c>
+      <c r="S48">
+        <f>MAX(R47-S47,S47-Q47)</f>
+        <v>0.96000000000000796</v>
+      </c>
+      <c r="U48" t="s">
+        <v>1</v>
+      </c>
+      <c r="V48">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="W48">
+        <v>74.88</v>
+      </c>
+      <c r="Z48">
+        <f>MAX(Z47-X47,Y47-Z47)</f>
+        <v>0.58000000000001251</v>
+      </c>
+      <c r="AC48">
+        <f>MAX(AB47-AC47,AC47-AA47)</f>
+        <v>1.38333333333334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="C49">
+        <v>77.94</v>
+      </c>
+      <c r="K49" t="s">
+        <v>2</v>
+      </c>
+      <c r="L49">
+        <v>76.97</v>
+      </c>
+      <c r="M49">
+        <v>76.06</v>
+      </c>
+      <c r="U49" t="s">
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <v>78.06</v>
+      </c>
+      <c r="W49">
+        <v>77.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new thesis version and VilT results on EXCEL
</commit_message>
<xml_diff>
--- a/results_crossentropy.xlsx
+++ b/results_crossentropy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001149822\personal\teseMECD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534DDC98-9374-4DA4-996A-20434D031E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1049C6-CEC7-4AB9-8411-8A0E0FBC0050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>Type - Contrastive VILT new way 0.01</t>
   </si>
   <si>
-    <t>Type - Logical Augmentation VILT new way</t>
+    <t>Type - Logical Extension VILT new way</t>
   </si>
 </sst>
 </file>
@@ -955,10 +955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC7418E-5114-4E07-B454-35F017667A5A}">
-  <dimension ref="A1:AX84"/>
+  <dimension ref="A1:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2735,162 +2735,6 @@
         <v>74.78</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>35</v>
-      </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>10</v>
-      </c>
-      <c r="G71" t="s">
-        <v>7</v>
-      </c>
-      <c r="H71" t="s">
-        <v>11</v>
-      </c>
-      <c r="I71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <f>MIN(B72:B76)</f>
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <f>MAX(B72:B76)</f>
-        <v>0</v>
-      </c>
-      <c r="F72" t="e">
-        <f>AVERAGE(B72:B76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G72">
-        <f>MIN(C72:C76)</f>
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <f>MAX(C72:C76)</f>
-        <v>0</v>
-      </c>
-      <c r="I72" t="e">
-        <f>AVERAGE(C72:C76)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>1</v>
-      </c>
-      <c r="F73" t="e">
-        <f>MAX(F72-D72,E72-F72)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I73" t="e">
-        <f>MAX(H72-I72,I72-G72)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>36</v>
-      </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" t="s">
-        <v>8</v>
-      </c>
-      <c r="F76" t="s">
-        <v>10</v>
-      </c>
-      <c r="G76" t="s">
-        <v>7</v>
-      </c>
-      <c r="H76" t="s">
-        <v>11</v>
-      </c>
-      <c r="I76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <f>MIN(B77:B81)</f>
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <f>MAX(B77:B81)</f>
-        <v>0</v>
-      </c>
-      <c r="F77" t="e">
-        <f>AVERAGE(B77:B81)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G77">
-        <f>MIN(C77:C81)</f>
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <f>MAX(C77:C81)</f>
-        <v>0</v>
-      </c>
-      <c r="I77" t="e">
-        <f>AVERAGE(C77:C81)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>1</v>
-      </c>
-      <c r="F78" t="e">
-        <f>MAX(F77-D77,E77-F77)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I78" t="e">
-        <f>MAX(H77-I77,I77-G77)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>2</v>
-      </c>
-      <c r="H79" t="e">
-        <f>(F77+I77)/2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>37</v>
@@ -2983,6 +2827,198 @@
       </c>
       <c r="C84">
         <v>73.989999999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" t="s">
+        <v>7</v>
+      </c>
+      <c r="H86" t="s">
+        <v>11</v>
+      </c>
+      <c r="I86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>74.05</v>
+      </c>
+      <c r="C87">
+        <v>75.569999999999993</v>
+      </c>
+      <c r="D87">
+        <f>MIN(B87:B91)</f>
+        <v>74.05</v>
+      </c>
+      <c r="E87">
+        <f>MAX(B87:B91)</f>
+        <v>74.790000000000006</v>
+      </c>
+      <c r="F87">
+        <f>AVERAGE(B87:B91)</f>
+        <v>74.426666666666677</v>
+      </c>
+      <c r="G87">
+        <f>MIN(C87:C91)</f>
+        <v>73</v>
+      </c>
+      <c r="H87">
+        <f>MAX(C87:C91)</f>
+        <v>75.569999999999993</v>
+      </c>
+      <c r="I87">
+        <f>AVERAGE(C87:C91)</f>
+        <v>74.45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>74.44</v>
+      </c>
+      <c r="C88">
+        <v>74.78</v>
+      </c>
+      <c r="F88">
+        <f>MAX(F87-D87,E87-F87)</f>
+        <v>0.37666666666667936</v>
+      </c>
+      <c r="I88">
+        <f>MAX(H87-I87,I87-G87)</f>
+        <v>1.4500000000000028</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <v>74.790000000000006</v>
+      </c>
+      <c r="C89">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91" t="s">
+        <v>7</v>
+      </c>
+      <c r="H91" t="s">
+        <v>11</v>
+      </c>
+      <c r="I91" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>73.8</v>
+      </c>
+      <c r="C92">
+        <v>72.3</v>
+      </c>
+      <c r="D92">
+        <f>MIN(B92:B96)</f>
+        <v>73.8</v>
+      </c>
+      <c r="E92">
+        <f>MAX(B92:B96)</f>
+        <v>75.239999999999995</v>
+      </c>
+      <c r="F92">
+        <f>AVERAGE(B92:B96)</f>
+        <v>74.33</v>
+      </c>
+      <c r="G92">
+        <f>MIN(C92:C96)</f>
+        <v>72.3</v>
+      </c>
+      <c r="H92">
+        <f>MAX(C92:C96)</f>
+        <v>73</v>
+      </c>
+      <c r="I92">
+        <f>AVERAGE(C92:C96)</f>
+        <v>72.733333333333334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>75.239999999999995</v>
+      </c>
+      <c r="C93">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F93">
+        <f>MAX(F92-D92,E92-F92)</f>
+        <v>0.90999999999999659</v>
+      </c>
+      <c r="I93">
+        <f>MAX(H92-I92,I92-G92)</f>
+        <v>0.43333333333333712</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>73.95</v>
+      </c>
+      <c r="C94">
+        <v>73</v>
+      </c>
+      <c r="H94">
+        <f>(F92+I92)/2</f>
+        <v>73.531666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>